<commit_message>
Add four integration tests + fix EventRepositoryTest + edit documentation
</commit_message>
<xml_diff>
--- a/TESTDocs/Testidokumentaatio.xlsx
+++ b/TESTDocs/Testidokumentaatio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://haagahelia.sharepoint.com/teams/Tiimi1nrtit/Jaetut asiakirjat/General/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://haagahelia-my.sharepoint.com/personal/bhi277_myy_haaga-helia_fi/Documents/Ohjelmistoprojekti 1 - SOF005AS3A-3015/nat20-ticketguru/TESTDocs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB1C1266-2A00-40DD-94A1-1F46DE8B0AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{FB1C1266-2A00-40DD-94A1-1F46DE8B0AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B97B11E-AE40-4281-BBD2-EE5ED44C2FA6}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12990" yWindow="75" windowWidth="38610" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Testaus" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="99">
   <si>
     <t>ID</t>
   </si>
@@ -345,12 +345,24 @@
   <si>
     <t>IN PROGRESS</t>
   </si>
+  <si>
+    <t>GlobalExceptionHandlerTest</t>
+  </si>
+  <si>
+    <t>AddAndRemovePermissionToRoleTest</t>
+  </si>
+  <si>
+    <t>SearchSaleTest</t>
+  </si>
+  <si>
+    <t>MarkTicketAsUsedByBarcodeTest</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -433,7 +445,87 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -463,6 +555,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -470,9 +565,6 @@
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -492,46 +584,6 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -546,19 +598,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD825061-E2B1-4307-AD38-2E47710E2F7C}" name="Table1" displayName="Table1" ref="A1:J18" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" headerRowBorderDxfId="10">
-  <autoFilter ref="A1:J18" xr:uid="{DD825061-E2B1-4307-AD38-2E47710E2F7C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD825061-E2B1-4307-AD38-2E47710E2F7C}" name="Table1" displayName="Table1" ref="A1:J22" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19">
+  <autoFilter ref="A1:J22" xr:uid="{DD825061-E2B1-4307-AD38-2E47710E2F7C}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{1E44A9C2-D1D1-43E6-8C51-B8B2BB4759E1}" name="ID" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{1FC689A4-A530-4C90-ACC4-1879EF0121D1}" name="Nimi" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{1951272E-DD55-41BC-A703-4EC75BEEB2C8}" name="Tyyppi" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{5CFC7E12-3BA4-4B17-ACB8-B034DD3B38CE}" name="Kohde" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{E69146D0-A97E-45AF-BC25-8DFAC34B8C00}" name="Toimenpiteet" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{5FF99162-4D3D-4EEA-8949-482A1783CF28}" name="Odotettu tulos" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{4538F7A5-CF53-4158-A4B6-03607626B64C}" name="Tekijä" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{9DF0C9DD-F268-4AF5-8F05-C1314C23A872}" name="Status" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{076D8560-959A-45DD-B9B7-DB1B1F153720}" name="Kommentti" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{CEF1C1A6-7890-487F-9C86-3E22BE62D6B4}" name="Testin tyypin valinnan perustelut" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{1E44A9C2-D1D1-43E6-8C51-B8B2BB4759E1}" name="ID" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{1FC689A4-A530-4C90-ACC4-1879EF0121D1}" name="Nimi" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{1951272E-DD55-41BC-A703-4EC75BEEB2C8}" name="Tyyppi" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{5CFC7E12-3BA4-4B17-ACB8-B034DD3B38CE}" name="Kohde" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{E69146D0-A97E-45AF-BC25-8DFAC34B8C00}" name="Toimenpiteet" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{5FF99162-4D3D-4EEA-8949-482A1783CF28}" name="Odotettu tulos" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{4538F7A5-CF53-4158-A4B6-03607626B64C}" name="Tekijä" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{9DF0C9DD-F268-4AF5-8F05-C1314C23A872}" name="Status" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{076D8560-959A-45DD-B9B7-DB1B1F153720}" name="Kommentti" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{CEF1C1A6-7890-487F-9C86-3E22BE62D6B4}" name="Testin tyypin valinnan perustelut" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -881,27 +933,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31" customWidth="1"/>
     <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="63.28515625" customWidth="1"/>
     <col min="10" max="10" width="65.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -933,7 +985,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="60.75" thickTop="1">
+    <row r="2" spans="1:10" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -965,7 +1017,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -995,7 +1047,7 @@
       </c>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1027,7 +1079,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="30">
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1059,7 +1111,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="45">
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1091,7 +1143,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="45">
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1123,7 +1175,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="30">
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1155,7 +1207,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="60">
+    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1187,7 +1239,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1219,7 +1271,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="30">
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1251,7 +1303,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="30">
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1283,7 +1335,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="45">
+    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1315,7 +1367,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="60">
+    <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1347,7 +1399,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="60">
+    <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1379,7 +1431,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="105">
+    <row r="16" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1411,7 +1463,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="75">
+    <row r="17" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1443,7 +1495,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="90">
+    <row r="18" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1472,6 +1524,86 @@
       <c r="J18" s="4" t="s">
         <v>91</v>
       </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="3"/>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="3"/>
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I21" s="3"/>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I22" s="3"/>
+      <c r="J22" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1534,7 +1666,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>H2:H18</xm:sqref>
+          <xm:sqref>H2:H22</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1544,7 +1676,7 @@
           <x14:formula1>
             <xm:f>Aputaulukko!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H18</xm:sqref>
+          <xm:sqref>H2:H22</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1560,32 +1692,32 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" thickBot="1">
+    <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75" thickTop="1">
+    <row r="2" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>94</v>
       </c>
@@ -1811,13 +1943,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1DAD84D-DE6B-4CFC-BCB8-CA758877D140}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1DAD84D-DE6B-4CFC-BCB8-CA758877D140}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e24e31e0-f14f-4471-bfc6-3a0dd1900cbf"/>
+    <ds:schemaRef ds:uri="8633b3aa-8e60-4418-ac0f-f2bf948ca6ee"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A1F9DC1-CFBE-404D-81AA-49611DD65107}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A1F9DC1-CFBE-404D-81AA-49611DD65107}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e24e31e0-f14f-4471-bfc6-3a0dd1900cbf"/>
+    <ds:schemaRef ds:uri="8633b3aa-8e60-4418-ac0f-f2bf948ca6ee"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19F81509-5FFB-46C8-9889-8E8A68DFE96B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19F81509-5FFB-46C8-9889-8E8A68DFE96B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update README on testing, edit test doc, and bang head on the wall re:JUnit tests
</commit_message>
<xml_diff>
--- a/TESTDocs/Testidokumentaatio.xlsx
+++ b/TESTDocs/Testidokumentaatio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://haagahelia-my.sharepoint.com/personal/bhi277_myy_haaga-helia_fi/Documents/Ohjelmistoprojekti 1 - SOF005AS3A-3015/nat20-ticketguru/TESTDocs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{FB1C1266-2A00-40DD-94A1-1F46DE8B0AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B97B11E-AE40-4281-BBD2-EE5ED44C2FA6}"/>
+  <xr:revisionPtr revIDLastSave="115" documentId="8_{FB1C1266-2A00-40DD-94A1-1F46DE8B0AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2429CAD-0B12-4BA6-83D5-0916198FC113}"/>
   <bookViews>
-    <workbookView xWindow="12990" yWindow="75" windowWidth="38610" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Testaus" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="156">
   <si>
     <t>ID</t>
   </si>
@@ -357,12 +357,209 @@
   <si>
     <t>MarkTicketAsUsedByBarcodeTest</t>
   </si>
+  <si>
+    <t>Back-end</t>
+  </si>
+  <si>
+    <t>- The ticket salesperson sees all upcoming events and relevant information: date, time, and event name
+- The ticket salesperson sees the number of available tickets to an event</t>
+  </si>
+  <si>
+    <t>- The ticket salesperson can choose an event to show additional information (place, description, city, and ticket types)
+- The ticket salesperson can choose any number of tickets per type to be sold to the selected event
+- Tickets to fully booked events cannot be sold</t>
+  </si>
+  <si>
+    <t>- The ticket salesperson can print sold tickets
+- The printed ticket contains all relevant information: event, venue, ticket type, price per ticket, and unique code per ticket</t>
+  </si>
+  <si>
+    <t>- The ticket salesperson can search for a sold ticket using the unique code
+- The search results in all relevant information: sales event, time of purchase, event, ticket type, and price</t>
+  </si>
+  <si>
+    <t>- The ticket salesperson can cancel a ticket
+- A cancelled ticket can no longer be used at an event</t>
+  </si>
+  <si>
+    <t>- The event coordinator can edit certain information in an event, like description, maximum number of tickets, ticket types, or prices</t>
+  </si>
+  <si>
+    <t>UserStory1</t>
+  </si>
+  <si>
+    <t>UserStory2</t>
+  </si>
+  <si>
+    <t>UserStory3</t>
+  </si>
+  <si>
+    <t>UserStory4</t>
+  </si>
+  <si>
+    <t>UserStory5</t>
+  </si>
+  <si>
+    <t>UserStory6</t>
+  </si>
+  <si>
+    <t>UserStory7</t>
+  </si>
+  <si>
+    <t>UserStory8</t>
+  </si>
+  <si>
+    <t>UserStory9</t>
+  </si>
+  <si>
+    <t>UserStory10</t>
+  </si>
+  <si>
+    <t>UserStory11</t>
+  </si>
+  <si>
+    <t>UserStory12</t>
+  </si>
+  <si>
+    <t>UserStory13</t>
+  </si>
+  <si>
+    <t>UserStory14</t>
+  </si>
+  <si>
+    <t>- The event coordinator can create a new event with all relevant information (event name, time, place, description, city, ticket types, prices, and maximum number of tickets to be sold)
+- The event becomes visible to event coordinators and ticket salespersons with an accurate amount of tickets available</t>
+  </si>
+  <si>
+    <t>- The event coordinator sees sales reports (tickets sold by type, sums, and particular sales)</t>
+  </si>
+  <si>
+    <t>- The admin can create new users with all relevant information (bare minimum: e-mail address and password)
+- New users can log in</t>
+  </si>
+  <si>
+    <t>- The admin can delete users
+- Information about deleted users is only available for the admin user</t>
+  </si>
+  <si>
+    <t>- The admin can edit or users
+- Information about edited users is accurate</t>
+  </si>
+  <si>
+    <t>- The admin can add roles to users
+- Roles change accordingly
+- User rights are defined by their roles</t>
+  </si>
+  <si>
+    <t>- The admin can edit roles assigned to users
+- Roles change accordingly
+- User rights are defined by their roles</t>
+  </si>
+  <si>
+    <t>- The admin can demote roles from users
+- Roles change accordingly
+- User rights are defined by their roles</t>
+  </si>
+  <si>
+    <t>Ainoa tapa varmistaa käyttäjätarinan toimivuus käyttäjän näkökulmasta</t>
+  </si>
+  <si>
+    <t>Varmistetaan, että GlobalExceptionHandler toimii odotetusti</t>
+  </si>
+  <si>
+    <t>Varmistetaan, että tietyltä roolilta voidaan poistaa tai sille voidaan lisätä uusia lupia odotetusti</t>
+  </si>
+  <si>
+    <t>Varmistetaan, että tietty myyntitapahtuma voidaan hakea joko käyttäjän tai tekohetken tiedoilla</t>
+  </si>
+  <si>
+    <t>Varmista, että GlobalExceptionHandler luettelee oikeat vikakoodit</t>
+  </si>
+  <si>
+    <t>Lisää ja poista lupa tietyltä roolilta</t>
+  </si>
+  <si>
+    <t>Etsi myyntitapahtuma</t>
+  </si>
+  <si>
+    <t>Etsi ja merkitse lippu käytetyksi viivakoodin avulla</t>
+  </si>
+  <si>
+    <t>Varmistetaan, että lippu voidaan etsiä ja merkitä käytetyksi viivakoodia käyttämällä</t>
+  </si>
+  <si>
+    <t>Varmista, että lipunmyyjä näkee tapahtumat ja niiden liput</t>
+  </si>
+  <si>
+    <t>Varmista, että lipunmyyjä voi valita tapahtuman ja sen liput</t>
+  </si>
+  <si>
+    <t>Varmista, että lipunmyyjä voi tulostaa myydyn lipun</t>
+  </si>
+  <si>
+    <t>Etsi ja katsele myytyjä lippuja lipunmyyjänä</t>
+  </si>
+  <si>
+    <t>Peru myyty lippu lipunmyyjänä</t>
+  </si>
+  <si>
+    <t>Muokkaa tapahtuman tietoja tapahtumavastaavana</t>
+  </si>
+  <si>
+    <t>Luo uusi tapahtuma tapahtumavastaavana</t>
+  </si>
+  <si>
+    <t>Katsele myyntiraporttia tapahtumavastaavana</t>
+  </si>
+  <si>
+    <t>Muokkaa käyttäjää ylläpitäjänä</t>
+  </si>
+  <si>
+    <t>Lisää käyttäjälle rooli ylläpitäjänä</t>
+  </si>
+  <si>
+    <t>Muokkaa käyttäjän roolia ylläpitäjänä</t>
+  </si>
+  <si>
+    <t>Poista käyttäjän rooli ylläpitäjänä</t>
+  </si>
+  <si>
+    <t>Lisää uusi käyttäjä ylläpitäjänä</t>
+  </si>
+  <si>
+    <t>Poista käyttäjä ylläpitäjänä</t>
+  </si>
+  <si>
+    <t>- Verify that the GlobalExceptionHandler processes a MethodArgumentNotValidException correctly
+- Verify that the method returns a map of field names to their respective validation error messages</t>
+  </si>
+  <si>
+    <t>- Test adding a permission to a role (Success)
+- Test adding a permission to a role when that permission already exists (Fail)
+- Test removing a permission from a role (Success)
+- Test removing a permission from a role when that permission does not exist (Fail)</t>
+  </si>
+  <si>
+    <t>- Search for a Sale successfully (Success)
+- Search for a Sale without providing parameters (Fail)
+- Search for a Sale that does not exist (Fail)</t>
+  </si>
+  <si>
+    <t>Success/Fail</t>
+  </si>
+  <si>
+    <t>- Search for a Ticket by Barcode (Success)
+- Search for a Ticket by Barcode that does not exist (Fail)
+- Use a Ticket by Barcode (Success)
+- Use a Ticket that does not exist (Fail)
+- Use a Ticket that has already been used (Fail)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -374,6 +571,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -598,8 +801,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD825061-E2B1-4307-AD38-2E47710E2F7C}" name="Table1" displayName="Table1" ref="A1:J22" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19">
-  <autoFilter ref="A1:J22" xr:uid="{DD825061-E2B1-4307-AD38-2E47710E2F7C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD825061-E2B1-4307-AD38-2E47710E2F7C}" name="Table1" displayName="Table1" ref="A1:J36" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19">
+  <autoFilter ref="A1:J36" xr:uid="{DD825061-E2B1-4307-AD38-2E47710E2F7C}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{1E44A9C2-D1D1-43E6-8C51-B8B2BB4759E1}" name="ID" dataDxfId="17"/>
     <tableColumn id="9" xr3:uid="{1FC689A4-A530-4C90-ACC4-1879EF0121D1}" name="Nimi" dataDxfId="16"/>
@@ -933,10 +1136,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1525,87 +1728,584 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="3"/>
+      <c r="C19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="G19" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="4"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I19" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="3"/>
+      <c r="C20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>154</v>
+      </c>
       <c r="G20" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="4"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I20" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>154</v>
+      </c>
       <c r="G21" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="I21" s="3"/>
-      <c r="J21" s="4"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="3"/>
+      <c r="C22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>154</v>
+      </c>
       <c r="G22" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H22" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="I22" s="3"/>
-      <c r="J22" s="4"/>
+      <c r="I23" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>128</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1666,7 +2366,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>H2:H22</xm:sqref>
+          <xm:sqref>H2:H36</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1676,7 +2376,7 @@
           <x14:formula1>
             <xm:f>Aputaulukko!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H22</xm:sqref>
+          <xm:sqref>H2:H36</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1728,6 +2428,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e24e31e0-f14f-4471-bfc6-3a0dd1900cbf">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="8633b3aa-8e60-4418-ac0f-f2bf948ca6ee" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Asiakirja" ma:contentTypeID="0x010100E2AB02CADA333D4893B03BA866FF1A57" ma:contentTypeVersion="11" ma:contentTypeDescription="Luo uusi asiakirja." ma:contentTypeScope="" ma:versionID="83ddf6fde8dcdcb41e26b7d613586a85">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e24e31e0-f14f-4471-bfc6-3a0dd1900cbf" xmlns:ns3="8633b3aa-8e60-4418-ac0f-f2bf948ca6ee" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="759f207cf1c80fb5ef1cb41ce3aba493" ns2:_="" ns3:_="">
     <xsd:import namespace="e24e31e0-f14f-4471-bfc6-3a0dd1900cbf"/>
@@ -1922,27 +2642,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e24e31e0-f14f-4471-bfc6-3a0dd1900cbf">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="8633b3aa-8e60-4418-ac0f-f2bf948ca6ee" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19F81509-5FFB-46C8-9889-8E8A68DFE96B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A1F9DC1-CFBE-404D-81AA-49611DD65107}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e24e31e0-f14f-4471-bfc6-3a0dd1900cbf"/>
+    <ds:schemaRef ds:uri="8633b3aa-8e60-4418-ac0f-f2bf948ca6ee"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1DAD84D-DE6B-4CFC-BCB8-CA758877D140}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1959,23 +2678,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A1F9DC1-CFBE-404D-81AA-49611DD65107}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e24e31e0-f14f-4471-bfc6-3a0dd1900cbf"/>
-    <ds:schemaRef ds:uri="8633b3aa-8e60-4418-ac0f-f2bf948ca6ee"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19F81509-5FFB-46C8-9889-8E8A68DFE96B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Complete E2E testing + edit test docs + edit readme
</commit_message>
<xml_diff>
--- a/TESTDocs/Testidokumentaatio.xlsx
+++ b/TESTDocs/Testidokumentaatio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://haagahelia-my.sharepoint.com/personal/bhi277_myy_haaga-helia_fi/Documents/Ohjelmistoprojekti 1 - SOF005AS3A-3015/nat20-ticketguru/TESTDocs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="115" documentId="8_{FB1C1266-2A00-40DD-94A1-1F46DE8B0AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2429CAD-0B12-4BA6-83D5-0916198FC113}"/>
+  <xr:revisionPtr revIDLastSave="158" documentId="8_{FB1C1266-2A00-40DD-94A1-1F46DE8B0AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08FBB4E2-675B-4FD2-AC71-CAB2D7DB9AF9}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Testaus" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="163">
   <si>
     <t>ID</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>Kommentti</t>
-  </si>
-  <si>
-    <t>Testin tyypin valinnan perustelut</t>
   </si>
   <si>
     <t>TicketRestTest</t>
@@ -470,9 +467,6 @@
     <t>Varmistetaan, että tietyltä roolilta voidaan poistaa tai sille voidaan lisätä uusia lupia odotetusti</t>
   </si>
   <si>
-    <t>Varmistetaan, että tietty myyntitapahtuma voidaan hakea joko käyttäjän tai tekohetken tiedoilla</t>
-  </si>
-  <si>
     <t>Varmista, että GlobalExceptionHandler luettelee oikeat vikakoodit</t>
   </si>
   <si>
@@ -485,16 +479,7 @@
     <t>Etsi ja merkitse lippu käytetyksi viivakoodin avulla</t>
   </si>
   <si>
-    <t>Varmistetaan, että lippu voidaan etsiä ja merkitä käytetyksi viivakoodia käyttämällä</t>
-  </si>
-  <si>
     <t>Varmista, että lipunmyyjä näkee tapahtumat ja niiden liput</t>
-  </si>
-  <si>
-    <t>Varmista, että lipunmyyjä voi valita tapahtuman ja sen liput</t>
-  </si>
-  <si>
-    <t>Varmista, että lipunmyyjä voi tulostaa myydyn lipun</t>
   </si>
   <si>
     <t>Etsi ja katsele myytyjä lippuja lipunmyyjänä</t>
@@ -540,19 +525,56 @@
 - Test removing a permission from a role when that permission does not exist (Fail)</t>
   </si>
   <si>
-    <t>- Search for a Sale successfully (Success)
+    <t>Success/Fail</t>
+  </si>
+  <si>
+    <t>Valitse tapahtuma ja sen liput lipunmyyjänä</t>
+  </si>
+  <si>
+    <t>Tulosta myyty lippu lipunmyyjänä</t>
+  </si>
+  <si>
+    <t>- Search for a Sale successfully (Success - NOK)
 - Search for a Sale without providing parameters (Fail)
 - Search for a Sale that does not exist (Fail)</t>
   </si>
   <si>
-    <t>Success/Fail</t>
-  </si>
-  <si>
-    <t>- Search for a Ticket by Barcode (Success)
+    <t>- Search for a Ticket by Barcode (Success - NOK)
 - Search for a Ticket by Barcode that does not exist (Fail)
-- Use a Ticket by Barcode (Success)
+- Use a Ticket by Barcode (Success - NOK)
 - Use a Ticket that does not exist (Fail)
 - Use a Ticket that has already been used (Fail)</t>
+  </si>
+  <si>
+    <t>UserStory15</t>
+  </si>
+  <si>
+    <t>Tarkastele lokeja ja järjestelmäraportteja ylläpitäjänä</t>
+  </si>
+  <si>
+    <t>Ei implementoitu</t>
+  </si>
+  <si>
+    <t>- The admin can see logs
+- The admin can see system reports</t>
+  </si>
+  <si>
+    <t>Varmistetaan, että tietty myyntitapahtuma voidaan hakea joko käyttäjän tai tekohetken tiedoilla. Ei saatu täysin toimimaan</t>
+  </si>
+  <si>
+    <t>Varmistetaan, että lippu voidaan etsiä ja merkitä käytetyksi viivakoodia käyttämällä. Ei saatu täysin toimimaan</t>
+  </si>
+  <si>
+    <t>Lipunmyyjä ei voi peruuttaa jo myytyä lippua</t>
+  </si>
+  <si>
+    <t>Tapahtumavastaava ei näe myyntiraportteja</t>
+  </si>
+  <si>
+    <t>Admin voi luoda uuden käyttäjän, mutta uusi käyttäjä ei pääse kirjautumaan järjestelmään</t>
+  </si>
+  <si>
+    <t>Vaiheet</t>
   </si>
 </sst>
 </file>
@@ -801,8 +823,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD825061-E2B1-4307-AD38-2E47710E2F7C}" name="Table1" displayName="Table1" ref="A1:J36" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19">
-  <autoFilter ref="A1:J36" xr:uid="{DD825061-E2B1-4307-AD38-2E47710E2F7C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD825061-E2B1-4307-AD38-2E47710E2F7C}" name="Table1" displayName="Table1" ref="A1:J37" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19">
+  <autoFilter ref="A1:J37" xr:uid="{DD825061-E2B1-4307-AD38-2E47710E2F7C}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{1E44A9C2-D1D1-43E6-8C51-B8B2BB4759E1}" name="ID" dataDxfId="17"/>
     <tableColumn id="9" xr3:uid="{1FC689A4-A530-4C90-ACC4-1879EF0121D1}" name="Nimi" dataDxfId="16"/>
@@ -812,8 +834,8 @@
     <tableColumn id="5" xr3:uid="{5FF99162-4D3D-4EEA-8949-482A1783CF28}" name="Odotettu tulos" dataDxfId="12"/>
     <tableColumn id="6" xr3:uid="{4538F7A5-CF53-4158-A4B6-03607626B64C}" name="Tekijä" dataDxfId="11"/>
     <tableColumn id="7" xr3:uid="{9DF0C9DD-F268-4AF5-8F05-C1314C23A872}" name="Status" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{076D8560-959A-45DD-B9B7-DB1B1F153720}" name="Kommentti" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{CEF1C1A6-7890-487F-9C86-3E22BE62D6B4}" name="Testin tyypin valinnan perustelut" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{076D8560-959A-45DD-B9B7-DB1B1F153720}" name="Vaiheet" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{CEF1C1A6-7890-487F-9C86-3E22BE62D6B4}" name="Kommentti" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1136,10 +1158,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1182,10 +1204,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1193,31 +1215,31 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="F2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="H2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1225,28 +1247,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>23</v>
       </c>
       <c r="J3" s="4"/>
     </row>
@@ -1255,31 +1277,31 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="8" t="s">
+      <c r="J4" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1287,31 +1309,31 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>32</v>
-      </c>
       <c r="J5" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1319,31 +1341,31 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="6" t="s">
+      <c r="J6" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1351,31 +1373,31 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="3" t="s">
+      <c r="J7" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1383,31 +1405,31 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="8" t="s">
+      <c r="J8" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1415,31 +1437,31 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="E9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="8" t="s">
+      <c r="J9" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1447,31 +1469,31 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="F10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="8" t="s">
+      <c r="J10" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1479,31 +1501,31 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="F11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" s="6" t="s">
+      <c r="J11" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1511,31 +1533,31 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="4" t="s">
+      <c r="F12" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="G12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="3" t="s">
+      <c r="J12" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1543,31 +1565,31 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="4" t="s">
+      <c r="F13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="6" t="s">
+      <c r="J13" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1575,31 +1597,31 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="4" t="s">
+      <c r="F14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I14" s="6" t="s">
+      <c r="J14" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1607,31 +1629,31 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="4" t="s">
+      <c r="F15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I15" s="6" t="s">
+      <c r="J15" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -1639,31 +1661,31 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="4" t="s">
+      <c r="F16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I16" s="6" t="s">
+      <c r="J16" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1671,31 +1693,31 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="4" t="s">
+      <c r="F17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I17" s="6" t="s">
+      <c r="J17" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -1704,28 +1726,28 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E18" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I18" s="6" t="s">
+      <c r="J18" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1733,31 +1755,31 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="H19" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -1765,31 +1787,31 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1797,31 +1819,31 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>131</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1829,31 +1851,31 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="E22" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1861,31 +1883,31 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G23" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="H23" s="3" t="s">
-        <v>94</v>
+        <v>15</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1893,127 +1915,121 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="F24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="H24" s="3" t="s">
-        <v>94</v>
+        <v>15</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>128</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="J24" s="4"/>
     </row>
     <row r="25" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="F25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G25" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="H25" s="3" t="s">
-        <v>94</v>
+        <v>15</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>128</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="J25" s="4"/>
     </row>
     <row r="26" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G26" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="H26" s="3" t="s">
-        <v>94</v>
+        <v>15</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>128</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="J26" s="4"/>
     </row>
     <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G27" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="H27" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>128</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2021,95 +2037,91 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G28" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="H28" s="3" t="s">
-        <v>94</v>
+        <v>15</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>128</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="J28" s="4"/>
     </row>
     <row r="29" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G29" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="H29" s="3" t="s">
-        <v>94</v>
+        <v>15</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>128</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="J29" s="4"/>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G30" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="H30" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2117,31 +2129,31 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G31" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="H31" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>128</v>
+        <v>161</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2149,159 +2161,181 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="F32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G32" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="H32" s="3" t="s">
-        <v>94</v>
+        <v>15</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>128</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="J32" s="4"/>
     </row>
     <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G33" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="H33" s="3" t="s">
-        <v>94</v>
+        <v>15</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>128</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="J33" s="4"/>
     </row>
     <row r="34" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G34" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="H34" s="3" t="s">
-        <v>94</v>
+        <v>15</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="J34" s="4" t="s">
-        <v>128</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="J34" s="4"/>
     </row>
     <row r="35" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G35" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="H35" s="3" t="s">
-        <v>94</v>
+        <v>15</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>128</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="J35" s="4"/>
     </row>
     <row r="36" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="F36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G36" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="H36" s="3" t="s">
-        <v>94</v>
+        <v>15</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
+      </c>
+      <c r="J36" s="4"/>
+    </row>
+    <row r="37" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -2366,7 +2400,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>H2:H36</xm:sqref>
+          <xm:sqref>H2:H37</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2376,7 +2410,7 @@
           <x14:formula1>
             <xm:f>Aputaulukko!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H36</xm:sqref>
+          <xm:sqref>H2:H37</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2404,22 +2438,22 @@
     </row>
     <row r="2" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>